<commit_message>
j,k columns removal communication header fixed adding customer and conference fields
</commit_message>
<xml_diff>
--- a/common/Travel Report Template.xlsx
+++ b/common/Travel Report Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,15 +19,15 @@
   <definedNames>
     <definedName name="Departments">גיליון2!$A$3:$A$7</definedName>
     <definedName name="depts.">גיליון2!$A$3:$A$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">גיליון1!$A$1:$J$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">גיליון1!$A$1:$I$48</definedName>
     <definedName name="Sales">גיליון2!$A$3:$A$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Travel #</t>
   </si>
@@ -104,18 +104,12 @@
     <t>$65 per day</t>
   </si>
   <si>
-    <t>Payment Method</t>
-  </si>
-  <si>
     <t>Restaurant</t>
   </si>
   <si>
     <t>Travel Insurance</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Bookkeeping account</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>Currency rate EURO</t>
   </si>
   <si>
-    <t>IF RELEVANT</t>
-  </si>
-  <si>
     <t>Department VP's Signature</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
   </si>
   <si>
     <t>Diesenhaus invoice</t>
-  </si>
-  <si>
-    <t>Transfer to Diesenhaus</t>
   </si>
   <si>
     <t>Details (non USD currency, if relevant)</t>
@@ -230,10 +218,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;?_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
@@ -243,7 +231,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -272,7 +260,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -280,7 +268,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -360,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -805,77 +793,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -921,10 +838,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -945,11 +862,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="2"/>
     </xf>
@@ -962,14 +879,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -983,21 +894,6 @@
     <xf numFmtId="168" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1023,18 +919,18 @@
     <xf numFmtId="167" fontId="8" fillId="6" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="6" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="6" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="8" fillId="5" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="8" fillId="5" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="8" fillId="5" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="8" fillId="5" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="5" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="8" fillId="5" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1057,12 +953,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="2" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="8" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1081,83 +972,118 @@
     <xf numFmtId="167" fontId="8" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="8" fillId="6" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1167,65 +1093,23 @@
     <xf numFmtId="2" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1322,23 +1206,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1374,23 +1241,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1570,44 +1420,40 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33:I33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="40.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="132" t="s">
+    <row r="1" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1617,12 +1463,10 @@
       <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="H2" s="26"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1632,22 +1476,20 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="51"/>
+      <c r="C4" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
@@ -1657,141 +1499,119 @@
       <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="G5" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="52"/>
+      <c r="C6" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="43"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="56"/>
-      <c r="I6" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="G6" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="52">
+      <c r="C7" s="43">
         <v>1</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="G7" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="H7" s="47"/>
+      <c r="I7" s="48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="56"/>
-      <c r="I8" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="G8" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="G9" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1801,29 +1621,25 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
+      <c r="C13" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1833,10 +1649,8 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1846,10 +1660,8 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1859,25 +1671,21 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="133" t="s">
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="134"/>
-      <c r="H17" s="134"/>
-      <c r="I17" s="134"/>
-      <c r="J17" s="135"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="108"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1887,331 +1695,287 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+    </row>
+    <row r="20" spans="1:9" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="29" t="s">
-        <v>47</v>
+      <c r="C20" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="129" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="130"/>
-      <c r="I20" s="131"/>
-      <c r="J20" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="128" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="129"/>
+      <c r="I20" s="130"/>
+    </row>
+    <row r="21" spans="1:9" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="60" t="e">
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51" t="e">
         <f t="shared" ref="D21:D26" si="0">C21*$I$5</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="108" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="109"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="107"/>
-      <c r="B22" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="105" t="s">
+      <c r="E21" s="51"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="110"/>
+      <c r="I21" s="111"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="94"/>
+      <c r="B22" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="60" t="e">
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="51" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E23" s="76"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="137"/>
-      <c r="I23" s="138"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="106"/>
-      <c r="B24" s="70"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="64" t="e">
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="114"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="127"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="55" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E24" s="72"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="139"/>
-      <c r="H24" s="140"/>
-      <c r="I24" s="141"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+      <c r="E24" s="63"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="115"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="117"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="31">
+      <c r="C25" s="29">
         <f>65*C11</f>
         <v>0</v>
       </c>
-      <c r="D25" s="33" t="e">
+      <c r="D25" s="31" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="37" t="e">
+      <c r="E25" s="32"/>
+      <c r="F25" s="35" t="e">
         <f>D25</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G25" s="120" t="s">
+      <c r="G25" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="121"/>
-      <c r="I25" s="122"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" s="104" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="105" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="94" t="s">
+      <c r="H25" s="119"/>
+      <c r="I25" s="120"/>
+    </row>
+    <row r="26" spans="1:9" s="90" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="95"/>
-      <c r="D26" s="96" t="e">
+      <c r="C26" s="83"/>
+      <c r="D26" s="84" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E26" s="96"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="144"/>
-      <c r="H26" s="145"/>
-      <c r="I26" s="146"/>
-      <c r="J26" s="102"/>
-      <c r="K26" s="103"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="107"/>
-      <c r="B27" s="30" t="s">
+      <c r="E26" s="84"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="96"/>
+      <c r="I26" s="97"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="94"/>
+      <c r="B27" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="124"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" s="84" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="150" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="78" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="79" t="e">
+      <c r="C27" s="30"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="121"/>
+      <c r="H27" s="122"/>
+      <c r="I27" s="123"/>
+    </row>
+    <row r="28" spans="1:9" s="73" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="70" t="e">
         <f>D28/I5</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="128"/>
-      <c r="J28" s="82"/>
-      <c r="K28" s="83"/>
-    </row>
-    <row r="29" spans="1:11" s="84" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="151"/>
-      <c r="B29" s="86" t="s">
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="125"/>
+      <c r="I28" s="126"/>
+    </row>
+    <row r="29" spans="1:9" s="73" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="105"/>
+      <c r="B29" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="117"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="119"/>
-      <c r="J29" s="85"/>
-      <c r="K29" s="83"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="30"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="135"/>
+      <c r="I29" s="136"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B30" s="11"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="115"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="90" t="s">
+      <c r="C30" s="76"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="99"/>
+      <c r="I30" s="100"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="91"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="147"/>
-      <c r="H31" s="148"/>
-      <c r="I31" s="149"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="105" t="s">
+      <c r="B31" s="79"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="102"/>
+      <c r="I31" s="103"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="94" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="95"/>
-      <c r="D32" s="96" t="e">
+      <c r="B32" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="83"/>
+      <c r="D32" s="84" t="e">
         <f>C32*$I$5</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E32" s="96"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="144"/>
-      <c r="H32" s="145"/>
-      <c r="I32" s="146"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="3"/>
-    </row>
-    <row r="33" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="106"/>
-      <c r="B33" s="98" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="99"/>
-      <c r="D33" s="100" t="e">
+      <c r="E32" s="84"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="95"/>
+      <c r="H32" s="96"/>
+      <c r="I32" s="97"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="127"/>
+      <c r="B33" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="87"/>
+      <c r="D33" s="88" t="e">
         <f>C33*$I$5</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E33" s="100"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="108" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" s="109"/>
-      <c r="I33" s="110"/>
-      <c r="J33" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="K33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="107"/>
-      <c r="B34" s="30" t="s">
+      <c r="E33" s="88"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="110"/>
+      <c r="I33" s="111"/>
+    </row>
+    <row r="34" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="94"/>
+      <c r="B34" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="112"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="3"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="30"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="131"/>
+      <c r="H34" s="132"/>
+      <c r="I34" s="133"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="39" t="e">
+      <c r="C35" s="37" t="e">
         <f>SUM(C21:C26)+SUM(C28:C28)+SUM(C30:C33)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D35" s="39" t="e">
+      <c r="D35" s="37" t="e">
         <f>SUM(D21:D26)+SUM(D28:D28)+SUM(D30:D33)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="37">
         <f>SUM(E21:E26)+SUM(E28:E28)+SUM(E30:E33)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="39" t="e">
+      <c r="F35" s="37" t="e">
         <f>SUM(F21:F26)+SUM(F28:F28)+SUM(F30:F33)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G35" s="114"/>
-      <c r="H35" s="115"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="3"/>
-    </row>
-    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="G35" s="98"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="100"/>
+    </row>
+    <row r="36" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2224,10 +1988,8 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-    </row>
-    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2237,10 +1999,8 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>20</v>
       </c>
@@ -2254,10 +2014,8 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -2272,10 +2030,8 @@
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-    </row>
-    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2285,10 +2041,8 @@
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-    </row>
-    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2298,29 +2052,25 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-    </row>
-    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="143" t="s">
+      <c r="E42" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="143"/>
-      <c r="G42" s="143"/>
+      <c r="F42" s="92"/>
+      <c r="G42" s="92"/>
       <c r="H42" s="5"/>
-      <c r="I42" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="J42" s="28"/>
-      <c r="K42" s="3"/>
-    </row>
-    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="I42" s="41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -2330,10 +2080,8 @@
       <c r="G43" s="21"/>
       <c r="H43" s="5"/>
       <c r="I43" s="19"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-    </row>
-    <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -2343,10 +2091,8 @@
       <c r="G44" s="6"/>
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-    </row>
-    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2356,10 +2102,8 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-    </row>
-    <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2369,43 +2113,37 @@
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="22"/>
       <c r="B47" s="23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
       <c r="H47" s="23"/>
       <c r="I47" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J47" s="23"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="22"/>
-      <c r="B48" s="48"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="23"/>
       <c r="D48" s="23"/>
-      <c r="E48" s="142"/>
-      <c r="F48" s="142"/>
-      <c r="G48" s="142"/>
+      <c r="E48" s="91"/>
+      <c r="F48" s="91"/>
+      <c r="G48" s="91"/>
       <c r="H48" s="23"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="I48" s="39"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="22"/>
       <c r="B49" s="23"/>
       <c r="C49" s="23"/>
@@ -2415,12 +2153,21 @@
       <c r="G49" s="23"/>
       <c r="H49" s="23"/>
       <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="24"/>
-      <c r="L49" s="2"/>
+      <c r="J49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="A26:A27"/>
@@ -2429,17 +2176,6 @@
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="G32:I32"/>
     <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="G20:I20"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="G33:I33"/>
     <mergeCell ref="G34:I34"/>
@@ -2459,7 +2195,7 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2472,7 +2208,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>